<commit_message>
update data & special thanks
</commit_message>
<xml_diff>
--- a/data/specialthanks.xlsx
+++ b/data/specialthanks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84694\Desktop\人生重来\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CFF8DE-5306-42A7-9046-C645220B4389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFC2E7A-DF07-4D67-9685-B7C370D39E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="180">
   <si>
     <t>$id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -190,10 +190,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>爱发电用户_4KcF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>胖罐子胖摔</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -466,6 +462,286 @@
   </si>
   <si>
     <t>leavatain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>南溪潇湘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弥夏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>午安僵尸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抹茶菠萝包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>血溅未央</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>千层蛋糕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>零下热情</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>作者真给力，游戏真稀奇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>淼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>呆了个呆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天一方</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰棍雪糕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>番茄一碗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我也不知道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>江子川</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>嘿嘿567</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Undead恩赐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>安德拉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爷只想要修仙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rua宝rua宝rua</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>变成光出轨奶琳小姐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二哥没牛子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>活在梦里</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>胖贼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wairy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>尨图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哆啦xzx梦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>符狸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吾名洛尉迟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全体目光向我看齐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>墨水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lkaiser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sky_sam</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 鱿鱼有了忧郁症很犹豫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没人要的瓜娃子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>六道神</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Incubator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雨溟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>印记</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>草帽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好大只36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MissVIP_ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拂晓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清岗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红尘多情客</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Akily</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工具人老衲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小爱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>羊296</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轻幻幻啊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brinter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>俗人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我大哥瀚青青</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>233号咸鱼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leeeooo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nybama</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿泰格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>特别感谢媳妇对我事业的支持。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">⁣​ </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老茶树菇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>若真的可以重来，那这次人生的意义不就变了吗？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爱发电用户_fUH5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Autumn_Loveworld</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果可以，请拾起年少时的幻想与疯狂，那是生活不曾亏待于我们的证明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bronies,bronies everywhere.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPCC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白微瑕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>瓜皮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>祝国内各位有梦想的独立游戏制作人一切顺利</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -797,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="D176" sqref="D176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -941,7 +1217,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -996,7 +1272,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1043,7 +1319,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1087,7 +1363,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1109,7 +1385,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1142,10 +1418,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1288,7 +1564,7 @@
         <v>2</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>41</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1299,7 +1575,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1310,7 +1586,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1321,7 +1597,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1332,7 +1608,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1343,7 +1619,7 @@
         <v>2</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1365,7 +1641,7 @@
         <v>2</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1376,7 +1652,7 @@
         <v>2</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1387,7 +1663,7 @@
         <v>2</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1398,7 +1674,7 @@
         <v>2</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1409,7 +1685,7 @@
         <v>2</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1420,7 +1696,7 @@
         <v>2</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1431,7 +1707,7 @@
         <v>2</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1442,7 +1718,7 @@
         <v>2</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1453,7 +1729,7 @@
         <v>2</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1464,7 +1740,7 @@
         <v>2</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1475,7 +1751,7 @@
         <v>2</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1486,7 +1762,7 @@
         <v>2</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1497,7 +1773,7 @@
         <v>2</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1508,7 +1784,7 @@
         <v>2</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1519,10 +1795,10 @@
         <v>2</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -1530,10 +1806,10 @@
         <v>2</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -1541,10 +1817,10 @@
         <v>2</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -1552,10 +1828,10 @@
         <v>2</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -1563,10 +1839,10 @@
         <v>2</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -1574,10 +1850,10 @@
         <v>2</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -1585,10 +1861,10 @@
         <v>2</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -1596,10 +1872,10 @@
         <v>2</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -1607,10 +1883,10 @@
         <v>2</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -1618,10 +1894,10 @@
         <v>2</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -1629,10 +1905,10 @@
         <v>2</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -1640,10 +1916,10 @@
         <v>2</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -1651,21 +1927,24 @@
         <v>2</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -1673,10 +1952,10 @@
         <v>2</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -1684,10 +1963,10 @@
         <v>2</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -1695,7 +1974,7 @@
         <v>2</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1706,7 +1985,7 @@
         <v>2</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1717,7 +1996,7 @@
         <v>2</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1728,10 +2007,10 @@
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1742,7 +2021,7 @@
         <v>2</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1753,7 +2032,7 @@
         <v>2</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1764,7 +2043,7 @@
         <v>2</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1775,7 +2054,7 @@
         <v>2</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1786,7 +2065,7 @@
         <v>2</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -1797,7 +2076,7 @@
         <v>2</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1808,7 +2087,7 @@
         <v>2</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -1819,7 +2098,7 @@
         <v>2</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -1830,7 +2109,7 @@
         <v>2</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1841,7 +2120,7 @@
         <v>2</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -1852,7 +2131,7 @@
         <v>2</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -1863,7 +2142,7 @@
         <v>2</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -1874,10 +2153,10 @@
         <v>2</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -1885,10 +2164,10 @@
         <v>2</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -1896,10 +2175,10 @@
         <v>2</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -1907,10 +2186,10 @@
         <v>2</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -1918,10 +2197,10 @@
         <v>2</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -1929,10 +2208,10 @@
         <v>2</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -1940,10 +2219,10 @@
         <v>2</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -1951,10 +2230,10 @@
         <v>2</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -1962,10 +2241,10 @@
         <v>2</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -1973,7 +2252,715 @@
         <v>2</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>104</v>
+      </c>
+      <c r="B106" s="1">
+        <v>2</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>105</v>
+      </c>
+      <c r="B107" s="1">
+        <v>2</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>106</v>
+      </c>
+      <c r="B108" s="1">
+        <v>2</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>107</v>
+      </c>
+      <c r="B109" s="1">
+        <v>2</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>108</v>
+      </c>
+      <c r="B110" s="1">
+        <v>2</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>109</v>
+      </c>
+      <c r="B111" s="1">
+        <v>1</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>110</v>
+      </c>
+      <c r="B112" s="1">
+        <v>1</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>111</v>
+      </c>
+      <c r="B113" s="1">
+        <v>2</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>112</v>
+      </c>
+      <c r="B114" s="1">
+        <v>2</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>113</v>
+      </c>
+      <c r="B115" s="1">
+        <v>2</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>114</v>
+      </c>
+      <c r="B116" s="1">
+        <v>2</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>115</v>
+      </c>
+      <c r="B117" s="1">
+        <v>2</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>116</v>
+      </c>
+      <c r="B118" s="1">
+        <v>2</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>117</v>
+      </c>
+      <c r="B119" s="1">
+        <v>2</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>118</v>
+      </c>
+      <c r="B120" s="1">
+        <v>2</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>119</v>
+      </c>
+      <c r="B121" s="1">
+        <v>2</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>120</v>
+      </c>
+      <c r="B122" s="1">
+        <v>2</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>121</v>
+      </c>
+      <c r="B123" s="1">
+        <v>2</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>122</v>
+      </c>
+      <c r="B124" s="1">
+        <v>2</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>123</v>
+      </c>
+      <c r="B125" s="1">
+        <v>2</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>124</v>
+      </c>
+      <c r="B126" s="1">
+        <v>2</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>125</v>
+      </c>
+      <c r="B127" s="1">
+        <v>2</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>126</v>
+      </c>
+      <c r="B128" s="1">
+        <v>2</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>127</v>
+      </c>
+      <c r="B129" s="1">
+        <v>2</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>128</v>
+      </c>
+      <c r="B130" s="1">
+        <v>2</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>129</v>
+      </c>
+      <c r="B131" s="1">
+        <v>2</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>130</v>
+      </c>
+      <c r="B132" s="1">
+        <v>2</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>131</v>
+      </c>
+      <c r="B133" s="1">
+        <v>2</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>132</v>
+      </c>
+      <c r="B134" s="1">
+        <v>2</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>133</v>
+      </c>
+      <c r="B135" s="1">
+        <v>2</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>134</v>
+      </c>
+      <c r="B136" s="1">
+        <v>2</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>135</v>
+      </c>
+      <c r="B137" s="1">
+        <v>2</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>136</v>
+      </c>
+      <c r="B138" s="1">
+        <v>2</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>137</v>
+      </c>
+      <c r="B139" s="1">
+        <v>2</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>138</v>
+      </c>
+      <c r="B140" s="1">
+        <v>2</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>139</v>
+      </c>
+      <c r="B141" s="1">
+        <v>2</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>140</v>
+      </c>
+      <c r="B142" s="1">
+        <v>2</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>141</v>
+      </c>
+      <c r="B143" s="1">
+        <v>1</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>142</v>
+      </c>
+      <c r="B144" s="1">
+        <v>2</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>143</v>
+      </c>
+      <c r="B145" s="1">
+        <v>2</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>144</v>
+      </c>
+      <c r="B146" s="1">
+        <v>2</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>145</v>
+      </c>
+      <c r="B147" s="1">
+        <v>2</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>146</v>
+      </c>
+      <c r="B148" s="1">
+        <v>2</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>147</v>
+      </c>
+      <c r="B149" s="1">
+        <v>2</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>148</v>
+      </c>
+      <c r="B150" s="1">
+        <v>2</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>149</v>
+      </c>
+      <c r="B151" s="1">
+        <v>2</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>150</v>
+      </c>
+      <c r="B152" s="1">
+        <v>2</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>151</v>
+      </c>
+      <c r="B153" s="1">
+        <v>2</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>152</v>
+      </c>
+      <c r="B154" s="1">
+        <v>2</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>153</v>
+      </c>
+      <c r="B155" s="1">
+        <v>2</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <v>154</v>
+      </c>
+      <c r="B156" s="1">
+        <v>2</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>155</v>
+      </c>
+      <c r="B157" s="1">
+        <v>2</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>156</v>
+      </c>
+      <c r="B158" s="1">
+        <v>2</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>157</v>
+      </c>
+      <c r="B159" s="1">
+        <v>2</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>158</v>
+      </c>
+      <c r="B160" s="1">
+        <v>2</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>159</v>
+      </c>
+      <c r="B161" s="1">
+        <v>2</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <v>160</v>
+      </c>
+      <c r="B162" s="1">
+        <v>2</v>
+      </c>
+      <c r="C162" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <v>161</v>
+      </c>
+      <c r="B163" s="1">
+        <v>2</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>162</v>
+      </c>
+      <c r="B164" s="1">
+        <v>1</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <v>163</v>
+      </c>
+      <c r="B165" s="1">
+        <v>2</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>164</v>
+      </c>
+      <c r="B166" s="1">
+        <v>2</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>165</v>
+      </c>
+      <c r="B167" s="1">
+        <v>2</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <v>166</v>
+      </c>
+      <c r="B168" s="1">
+        <v>1</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>